<commit_message>
some more fixes regarding fileNames in emails sent
</commit_message>
<xml_diff>
--- a/ans/result/1401CS40.xlsx
+++ b/ans/result/1401CS40.xlsx
@@ -96,13 +96,13 @@
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="4" numFmtId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="5" numFmtId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
@@ -120,13 +120,13 @@
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="7">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="6">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="7">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="5">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="4">
@@ -139,9 +139,9 @@
     <cellStyle hidden="0" name="ltitleStyle" xfId="2"/>
     <cellStyle hidden="0" name="mtitleStyle" xfId="3"/>
     <cellStyle hidden="0" name="absoluteStyle" xfId="4"/>
-    <cellStyle hidden="0" name="correctStyle" xfId="5"/>
-    <cellStyle hidden="0" name="incorrectStyle" xfId="6"/>
-    <cellStyle hidden="0" name="normalStyle" xfId="7"/>
+    <cellStyle hidden="0" name="normalStyle" xfId="5"/>
+    <cellStyle hidden="0" name="correctStyle" xfId="6"/>
+    <cellStyle hidden="0" name="incorrectStyle" xfId="7"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
@@ -623,13 +623,13 @@
         </is>
       </c>
       <c r="B10" s="5" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D10" s="7" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E10" s="7" t="n">
         <v>28</v>
@@ -661,15 +661,15 @@
         </is>
       </c>
       <c r="B12" s="5" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>-24</v>
+        <v>0</v>
       </c>
       <c r="D12" s="7" t="n"/>
       <c r="E12" s="8" t="inlineStr">
         <is>
-          <t>76/140</t>
+          <t>Absent</t>
         </is>
       </c>
     </row>
@@ -696,317 +696,209 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="inlineStr">
+      <c r="A16" s="7" t="inlineStr"/>
+      <c r="B16" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
-      <c r="B16" s="8" t="inlineStr">
+      <c r="D16" s="7" t="inlineStr"/>
+      <c r="E16" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
-      <c r="D16" s="5" t="inlineStr">
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr"/>
+      <c r="B17" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+      <c r="D17" s="7" t="inlineStr"/>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr"/>
+      <c r="B18" s="8" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+      <c r="D18" s="7" t="inlineStr"/>
+      <c r="E18" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr"/>
+      <c r="B19" s="8" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr"/>
+      <c r="B20" s="8" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="inlineStr"/>
+      <c r="B21" s="8" t="inlineStr">
+        <is>
+          <t>Option C</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="inlineStr"/>
+      <c r="B22" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="inlineStr"/>
+      <c r="B23" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="inlineStr"/>
+      <c r="B24" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
-      <c r="E16" s="8" t="inlineStr">
+    </row>
+    <row r="25">
+      <c r="A25" s="7" t="inlineStr"/>
+      <c r="B25" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="5" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="B17" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="D17" s="5" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="7" t="inlineStr"/>
+      <c r="B26" s="8" t="inlineStr">
         <is>
           <t>Option C</t>
         </is>
       </c>
-      <c r="E17" s="8" t="inlineStr">
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr"/>
+      <c r="B27" s="8" t="inlineStr">
+        <is>
+          <t>Option A</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="inlineStr"/>
+      <c r="B28" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="inlineStr"/>
+      <c r="B29" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="inlineStr"/>
+      <c r="B30" s="8" t="inlineStr">
+        <is>
+          <t>Option B</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="7" t="inlineStr"/>
+      <c r="B31" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="inlineStr"/>
+      <c r="B32" s="8" t="inlineStr">
         <is>
           <t>Option C</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="5" t="inlineStr">
+    <row r="33">
+      <c r="A33" s="7" t="inlineStr"/>
+      <c r="B33" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="7" t="inlineStr"/>
+      <c r="B34" s="8" t="inlineStr">
         <is>
           <t>Option B</t>
         </is>
       </c>
-      <c r="B18" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="D18" s="5" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="E18" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-      <c r="B19" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="B20" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-      <c r="B21" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="inlineStr">
+    </row>
+    <row r="35">
+      <c r="A35" s="7" t="inlineStr"/>
+      <c r="B35" s="8" t="inlineStr">
+        <is>
+          <t>Option D</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="7" t="inlineStr"/>
+      <c r="B36" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
-      <c r="B22" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="B23" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="B24" s="8" t="inlineStr">
+    </row>
+    <row r="37">
+      <c r="A37" s="7" t="inlineStr"/>
+      <c r="B37" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="5" t="inlineStr">
+    <row r="38">
+      <c r="A38" s="7" t="inlineStr"/>
+      <c r="B38" s="8" t="inlineStr">
         <is>
           <t>Option A</t>
         </is>
       </c>
-      <c r="B25" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="5" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-      <c r="B26" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="6" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-      <c r="B27" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="5" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="B28" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="5" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="B29" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="5" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="B30" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="6" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="B31" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="5" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-      <c r="B32" s="8" t="inlineStr">
-        <is>
-          <t>Option C</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="5" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="B33" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="6" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-      <c r="B34" s="8" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="6" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="B35" s="8" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="5" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-      <c r="B36" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="6" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
-      <c r="B37" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="5" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
-      <c r="B38" s="8" t="inlineStr">
-        <is>
-          <t>Option A</t>
-        </is>
-      </c>
     </row>
     <row r="39">
-      <c r="A39" s="5" t="inlineStr">
-        <is>
-          <t>Option D</t>
-        </is>
-      </c>
+      <c r="A39" s="7" t="inlineStr"/>
       <c r="B39" s="8" t="inlineStr">
         <is>
           <t>Option D</t>
@@ -1014,11 +906,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="6" t="inlineStr">
-        <is>
-          <t>Option B</t>
-        </is>
-      </c>
+      <c r="A40" s="7" t="inlineStr"/>
       <c r="B40" s="8" t="inlineStr">
         <is>
           <t>Option D</t>

</xml_diff>